<commit_message>
Added paper statistics processer
</commit_message>
<xml_diff>
--- a/LLMpaper_MetricsResults.xlsx
+++ b/LLMpaper_MetricsResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhi\Desktop\UTD-Projects\MedCruncher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F519459-A0B9-43EF-94BC-01DF1F4FB9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AE0AF4-F3C6-43D6-A591-BF131717267A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12504" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R1" sheetId="2" r:id="rId1"/>
@@ -245,15 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -267,6 +258,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF9C374-685C-44C7-A29F-17670034A493}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,7 +583,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -595,10 +595,10 @@
       <c r="D1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>27</v>
       </c>
       <c r="H1" t="s">
@@ -606,57 +606,57 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="13" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -668,36 +668,36 @@
       <c r="D9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="18"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -708,7 +708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -737,880 +737,893 @@
       <c r="F1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
       <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
+      <c r="A7" s="19">
         <v>2</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="19">
         <v>3</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
+      <c r="A17" s="19">
         <v>4</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="19" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
       <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="12">
+      <c r="A22" s="19">
         <v>5</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="12">
+      <c r="A27" s="19">
         <v>6</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="12">
+      <c r="A32" s="19">
         <v>7</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
       <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
       <c r="C34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
       <c r="C35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
       <c r="C36" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="12">
+      <c r="A37" s="19">
         <v>8</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="19"/>
+      <c r="B38" s="19"/>
       <c r="C38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="19"/>
       <c r="C39" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="19"/>
+      <c r="B40" s="19"/>
       <c r="C40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="19"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="12">
+      <c r="A42" s="19">
         <v>9</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="19"/>
+      <c r="B43" s="19"/>
       <c r="C43" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
       <c r="C44" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="19"/>
+      <c r="B45" s="19"/>
       <c r="C45" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" s="12">
+      <c r="A47" s="19">
         <v>10</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="19"/>
+      <c r="B48" s="19"/>
       <c r="C48" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
       <c r="C49" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
       <c r="C50" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
       <c r="C51" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="12">
+      <c r="A52" s="19">
         <v>11</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="17"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
+      <c r="A53" s="19"/>
+      <c r="B53" s="19"/>
       <c r="C53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D53" s="17"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="19"/>
       <c r="C54" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
+      <c r="A55" s="19"/>
+      <c r="B55" s="19"/>
       <c r="C55" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
+      <c r="A56" s="19"/>
+      <c r="B56" s="19"/>
       <c r="C56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="12">
+      <c r="A57" s="19">
         <v>12</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
       <c r="C58" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="12"/>
-      <c r="B59" s="12"/>
+      <c r="A59" s="19"/>
+      <c r="B59" s="19"/>
       <c r="C59" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="12"/>
-      <c r="B60" s="12"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
       <c r="C60" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A61" s="12"/>
-      <c r="B61" s="12"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
       <c r="C61" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="12">
+      <c r="A62" s="19">
         <v>13</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="12"/>
-      <c r="B63" s="12"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
       <c r="C63" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D63" s="17"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="12"/>
-      <c r="B64" s="12"/>
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D64" s="17"/>
-      <c r="E64" s="17"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A65" s="12"/>
-      <c r="B65" s="12"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
       <c r="C65" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A66" s="12"/>
-      <c r="B66" s="12"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="19"/>
       <c r="C66" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D66" s="17"/>
-      <c r="E66" s="17"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B67" s="14"/>
+      <c r="B67" s="20"/>
       <c r="C67" s="5"/>
       <c r="G67" s="3"/>
       <c r="H67" s="2"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B68" s="14"/>
+      <c r="B68" s="20"/>
       <c r="C68" s="5"/>
       <c r="G68" s="4"/>
       <c r="H68" s="2"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B69" s="14"/>
+      <c r="B69" s="20"/>
       <c r="C69" s="5"/>
       <c r="G69" s="4"/>
       <c r="H69" s="2"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B70" s="14"/>
+      <c r="B70" s="20"/>
       <c r="C70" s="5"/>
       <c r="G70" s="4"/>
       <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B71" s="14"/>
+      <c r="B71" s="20"/>
       <c r="C71" s="5"/>
       <c r="G71" s="4"/>
       <c r="H71" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A57:A61"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B47:B51"/>
     <mergeCell ref="B67:B71"/>
@@ -1625,19 +1638,6 @@
     <mergeCell ref="B57:B61"/>
     <mergeCell ref="B27:B31"/>
     <mergeCell ref="B52:B56"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A57:A61"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="A37:A41"/>
-    <mergeCell ref="A42:A46"/>
-    <mergeCell ref="A47:A51"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1648,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05508DA-7A93-4025-9DB3-C382921763A3}">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,349 +1677,331 @@
       <c r="F1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
       <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="18"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+      <c r="A4" s="19">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="19">
         <v>3</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="12">
+      <c r="A8" s="19">
         <v>4</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="19" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="12">
+      <c r="A10" s="19">
         <v>5</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="19" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
+      <c r="A12" s="19">
         <v>6</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
+      <c r="A14" s="19">
         <v>7</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="12">
+      <c r="A16" s="19">
         <v>8</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="1"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="12">
+      <c r="A18" s="19">
         <v>9</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="19" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="12">
+      <c r="A20" s="19">
         <v>10</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="19"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="12">
+      <c r="A22" s="19">
         <v>11</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="12">
+      <c r="A24" s="19">
         <v>12</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="19" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="12">
+      <c r="A26" s="19">
         <v>13</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="20"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="5"/>
       <c r="G28" s="3"/>
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="20"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="5"/>
       <c r="G29" s="4"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="20"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="5"/>
       <c r="G30" s="4"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="20"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="5"/>
       <c r="G31" s="4"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B32" s="20"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="5"/>
       <c r="G32" s="4"/>
       <c r="H32" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="A20:A21"/>
@@ -2028,6 +2010,24 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2035,15 +2035,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ADB76A50BFBD143874E0E8B8790C9A2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="052157b9451f08e2e16cb38c14804f12">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7d3cea92-af5d-48a9-9910-15a783d83ae5" xmlns:ns3="c917d6de-2663-4e70-8d83-a35ffdb68441" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c0476fe8f92bfd09c90bd98ebc1a330" ns2:_="" ns3:_="">
     <xsd:import namespace="7d3cea92-af5d-48a9-9910-15a783d83ae5"/>
@@ -2266,15 +2257,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADDCA5F8-DAF6-4CE9-BBE1-87B9ACC455CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97D7D5A1-D34A-4707-9618-471C337084F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2291,4 +2283,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADDCA5F8-DAF6-4CE9-BBE1-87B9ACC455CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Metrics and Diagrams Completed
</commit_message>
<xml_diff>
--- a/LLMpaper_MetricsResults.xlsx
+++ b/LLMpaper_MetricsResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhi\Desktop\GITHUB PROJECTS\MedCruncher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikhi\Desktop\UTD-Projects\MedCruncher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245F9631-C45B-4594-841A-68C4544C7A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF126B86-7BFD-43F8-B2A2-66A2C673E373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R1" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="327">
   <si>
     <t>Disease</t>
   </si>
@@ -974,13 +974,58 @@
   </si>
   <si>
     <t>0.9785 ± 0.0049</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>0.1796 ± 0.0432</t>
+  </si>
+  <si>
+    <t>0.9990 ± 0.0011</t>
+  </si>
+  <si>
+    <t>0.2526 ± 0.0542</t>
+  </si>
+  <si>
+    <t>0.0354 ± 0.0173</t>
+  </si>
+  <si>
+    <t>0.2261 ± 0.0443</t>
+  </si>
+  <si>
+    <t>0.1398 ± 0.0326</t>
+  </si>
+  <si>
+    <t>0.9347 ± 0.0097</t>
+  </si>
+  <si>
+    <t>0.9958 ± 0.0026</t>
+  </si>
+  <si>
+    <t>0.9454 ± 0.0104</t>
+  </si>
+  <si>
+    <t>0.9978 ± 0.0016</t>
+  </si>
+  <si>
+    <t>0.9396 ± 0.0074</t>
+  </si>
+  <si>
+    <t>0.9230 ± 0.0064</t>
+  </si>
+  <si>
+    <t>0.8875 ± 0.0094</t>
+  </si>
+  <si>
+    <t>0.9309 ± 0.0095</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1021,6 +1066,11 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1058,12 +1108,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1072,13 +1119,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1092,41 +1132,50 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1431,184 +1480,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF9C374-685C-44C7-A29F-17670034A493}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10"/>
+      <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="F2" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0.64200000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="F3" s="10">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="F4" s="21">
+        <v>7.5300000000000006E-8</v>
+      </c>
+      <c r="G4" s="21">
+        <v>1.84E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="F5" s="21">
+        <v>1.3300000000000001E-20</v>
+      </c>
+      <c r="G5" s="21">
+        <v>3.6600000000000002E-19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="10" t="s">
         <v>301</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="F6" s="10">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2.1700000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="10" t="s">
         <v>303</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="10" t="s">
         <v>304</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="10" t="s">
         <v>305</v>
       </c>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="F10" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="F11" s="10">
+        <v>0.25280000000000002</v>
+      </c>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="10" t="s">
         <v>309</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="F12" s="10">
+        <v>0.47010000000000002</v>
+      </c>
+      <c r="G12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1617,1303 +1741,1685 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B31"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="18.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="14" style="21" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="9"/>
+    <col min="1" max="1" width="5.5546875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="14" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H2" s="18">
+        <v>2.164704628492806E-5</v>
+      </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="15" t="s">
+      <c r="G3" s="10">
+        <v>2.164704628492806E-5</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="15" t="s">
+      <c r="G4" s="10">
+        <v>2.3013977990811302E-9</v>
+      </c>
+      <c r="H4" s="18">
+        <v>2.3013977990811302E-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="15" t="s">
+      <c r="G5" s="10">
+        <v>7.0239263725341187E-17</v>
+      </c>
+      <c r="H5" s="18">
+        <v>7.0239263725341187E-17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="G6" s="10">
+        <v>0.23507727008942261</v>
+      </c>
+      <c r="H6" s="18">
+        <v>0.23507727008942261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14">
         <v>2</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="15" t="s">
+      <c r="G7" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H7" s="18">
+        <v>6.580286203444298E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="15" t="s">
+      <c r="G8" s="10">
+        <v>6.580286203444298E-2</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="14"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="15" t="s">
+      <c r="G9" s="10">
+        <v>1.1889333726884119E-10</v>
+      </c>
+      <c r="H9" s="18">
+        <v>1.1889333726884119E-10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="14"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="15" t="s">
+      <c r="G10" s="10">
+        <v>1.683913181220523E-15</v>
+      </c>
+      <c r="H10" s="18">
+        <v>1.683913181220523E-15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="G11" s="10">
+        <v>1.026655849917441E-5</v>
+      </c>
+      <c r="H11" s="18">
+        <v>1.026655849917441E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
         <v>3</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="15" t="s">
+      <c r="G12" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H12" s="18">
+        <v>0.24246196166157091</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="15" t="s">
+      <c r="G13" s="10">
+        <v>0.24246196166157091</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="15" t="s">
+      <c r="G14" s="10">
+        <v>3.6065480950778072E-12</v>
+      </c>
+      <c r="H14" s="18">
+        <v>3.6065480950778072E-12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-    </row>
-    <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="15" t="s">
+      <c r="G15" s="10">
+        <v>2.0469415910074049E-17</v>
+      </c>
+      <c r="H15" s="18">
+        <v>2.0469415910074049E-17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-    </row>
-    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
+      <c r="G16" s="10">
+        <v>1.4121732312054519E-8</v>
+      </c>
+      <c r="H16" s="18">
+        <v>1.4121732312054519E-8</v>
+      </c>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
         <v>4</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-    </row>
-    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="15" t="s">
+      <c r="G17" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H17" s="18">
+        <v>2.6029868449572492E-4</v>
+      </c>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-    </row>
-    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="15" t="s">
+      <c r="G18" s="10">
+        <v>2.6029868449572492E-4</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="15" t="s">
+      <c r="G19" s="10">
+        <v>6.2396378019923972E-9</v>
+      </c>
+      <c r="H19" s="18">
+        <v>6.2396378019923972E-9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="15" t="s">
+      <c r="G20" s="10">
+        <v>2.7044155208812281E-19</v>
+      </c>
+      <c r="H20" s="18">
+        <v>2.7044155208812281E-19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
+      <c r="G21" s="10">
+        <v>0.20286942900441679</v>
+      </c>
+      <c r="H21" s="18">
+        <v>0.20286942900441679</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
         <v>5</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="15" t="s">
+      <c r="G22" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H22" s="18">
+        <v>1.5819620117150841E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-    </row>
-    <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="15" t="s">
+      <c r="G23" s="10">
+        <v>1.5819620117150841E-2</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-    </row>
-    <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="15" t="s">
+      <c r="G24" s="10">
+        <v>7.1622620580793064E-10</v>
+      </c>
+      <c r="H24" s="18">
+        <v>7.1622620580793064E-10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-    </row>
-    <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="15" t="s">
+      <c r="G25" s="10">
+        <v>6.6447712637474777E-19</v>
+      </c>
+      <c r="H25" s="18">
+        <v>6.6447712637474777E-19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="19" t="s">
         <v>200</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="19" t="s">
         <v>201</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-    </row>
-    <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
+      <c r="G26" s="10">
+        <v>0.2209947921742462</v>
+      </c>
+      <c r="H26" s="18">
+        <v>0.2209947921742462</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
         <v>6</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-    </row>
-    <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="15" t="s">
+      <c r="G27" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H27" s="18">
+        <v>4.9265200297589924E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-    </row>
-    <row r="29" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="15" t="s">
+      <c r="G28" s="10">
+        <v>4.9265200297589924E-3</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-    </row>
-    <row r="30" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="15" t="s">
+      <c r="G29" s="10">
+        <v>0.10723697354312541</v>
+      </c>
+      <c r="H29" s="18">
+        <v>0.10723697354312541</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-    </row>
-    <row r="31" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="15" t="s">
+      <c r="G30" s="10">
+        <v>9.9997606196686465E-7</v>
+      </c>
+      <c r="H30" s="18">
+        <v>9.9997606196686465E-7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-    </row>
-    <row r="32" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18">
+      <c r="G31" s="10">
+        <v>4.0226683885690411E-4</v>
+      </c>
+      <c r="H31" s="18">
+        <v>4.0226683885690411E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
         <v>7</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-    </row>
-    <row r="33" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="15" t="s">
+      <c r="G32" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H32" s="18">
+        <v>1.016257212069078E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-    </row>
-    <row r="34" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="15" t="s">
+      <c r="G33" s="10">
+        <v>1.016257212069078E-2</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-    </row>
-    <row r="35" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="15" t="s">
+      <c r="G34" s="10">
+        <v>1.241535982206754E-2</v>
+      </c>
+      <c r="H34" s="18">
+        <v>1.241535982206754E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-    </row>
-    <row r="36" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="15" t="s">
+      <c r="G35" s="10">
+        <v>4.8696389855756459E-7</v>
+      </c>
+      <c r="H35" s="18">
+        <v>4.8696389855756459E-7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-    </row>
-    <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18">
+      <c r="G36" s="10">
+        <v>1.483718290432734E-3</v>
+      </c>
+      <c r="H36" s="18">
+        <v>1.483718290432734E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
         <v>8</v>
       </c>
-      <c r="B37" s="24" t="s">
+      <c r="B37" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-    </row>
-    <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="15" t="s">
+      <c r="G37" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H37" s="18">
+        <v>2.2095175776121741E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-    </row>
-    <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="15" t="s">
+      <c r="G38" s="10">
+        <v>2.2095175776121741E-2</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-    </row>
-    <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="15" t="s">
+      <c r="G39" s="10">
+        <v>0.29172799620347251</v>
+      </c>
+      <c r="H39" s="18">
+        <v>0.29172799620347251</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-    </row>
-    <row r="41" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="15" t="s">
+      <c r="G40" s="10">
+        <v>1.47932919316272E-6</v>
+      </c>
+      <c r="H40" s="18">
+        <v>1.47932919316272E-6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-    </row>
-    <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18">
+      <c r="G41" s="10">
+        <v>0.15886984058331799</v>
+      </c>
+      <c r="H41" s="18">
+        <v>0.15886984058331799</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14">
         <v>9</v>
       </c>
-      <c r="B42" s="24" t="s">
+      <c r="B42" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="15" t="s">
+      <c r="G42" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H42" s="18">
+        <v>0.26065785143676101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-    </row>
-    <row r="44" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="15" t="s">
+      <c r="G43" s="10">
+        <v>0.26065785143676101</v>
+      </c>
+      <c r="H43" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="G44" s="16"/>
-      <c r="H44" s="16"/>
-    </row>
-    <row r="45" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="15" t="s">
+      <c r="G44" s="10">
+        <v>1.2364180708495131E-10</v>
+      </c>
+      <c r="H44" s="18">
+        <v>1.2364180708495131E-10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="14"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16"/>
-    </row>
-    <row r="46" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="15" t="s">
+      <c r="G45" s="10">
+        <v>2.8903878518725167E-14</v>
+      </c>
+      <c r="H45" s="18">
+        <v>2.8903878518725167E-14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-    </row>
-    <row r="47" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18">
+      <c r="G46" s="10">
+        <v>9.1222832404332896E-6</v>
+      </c>
+      <c r="H46" s="18">
+        <v>9.1222832404332896E-6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14">
         <v>10</v>
       </c>
-      <c r="B47" s="24" t="s">
+      <c r="B47" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-    </row>
-    <row r="48" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="15" t="s">
+      <c r="G47" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H47" s="18">
+        <v>0.10605708102959679</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="14"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-    </row>
-    <row r="49" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="15" t="s">
+      <c r="G48" s="10">
+        <v>0.10605708102959679</v>
+      </c>
+      <c r="H48" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="G49" s="16"/>
-      <c r="H49" s="16"/>
-    </row>
-    <row r="50" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="15" t="s">
+      <c r="G49" s="10">
+        <v>0.27024542979362021</v>
+      </c>
+      <c r="H49" s="18">
+        <v>0.27024542979362021</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="G50" s="16"/>
-      <c r="H50" s="16"/>
-    </row>
-    <row r="51" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="15" t="s">
+      <c r="G50" s="10">
+        <v>1.854211490309085E-4</v>
+      </c>
+      <c r="H50" s="18">
+        <v>1.854211490309085E-4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="14"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E51" s="15" t="s">
+      <c r="E51" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G51" s="16"/>
-      <c r="H51" s="16"/>
-    </row>
-    <row r="52" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="18">
+      <c r="G51" s="10">
+        <v>0.20088351180535161</v>
+      </c>
+      <c r="H51" s="18">
+        <v>0.20088351180535161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="14">
         <v>11</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-    </row>
-    <row r="53" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="15" t="s">
+      <c r="G52" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H52" s="18">
+        <v>2.0867737471232399E-5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E53" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16"/>
-    </row>
-    <row r="54" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="18"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="15" t="s">
+      <c r="G53" s="10">
+        <v>2.0867737471232399E-5</v>
+      </c>
+      <c r="H53" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="14"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="19" t="s">
         <v>259</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E54" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-    </row>
-    <row r="55" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="18"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="15" t="s">
+      <c r="G54" s="10">
+        <v>7.5667029724899644E-4</v>
+      </c>
+      <c r="H54" s="18">
+        <v>7.5667029724899644E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="14"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="E55" s="15" t="s">
+      <c r="E55" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="F55" s="15" t="s">
+      <c r="F55" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16"/>
-    </row>
-    <row r="56" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="15" t="s">
+      <c r="G55" s="10">
+        <v>4.2467929203188112E-12</v>
+      </c>
+      <c r="H55" s="18">
+        <v>4.2467929203188112E-12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="E56" s="15" t="s">
+      <c r="E56" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="F56" s="15" t="s">
+      <c r="F56" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
-    </row>
-    <row r="57" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="18">
+      <c r="G56" s="10">
+        <v>9.4104904334435882E-4</v>
+      </c>
+      <c r="H56" s="18">
+        <v>9.4104904334435882E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14">
         <v>12</v>
       </c>
-      <c r="B57" s="24" t="s">
+      <c r="B57" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E57" s="15" t="s">
+      <c r="E57" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F57" s="15" t="s">
+      <c r="F57" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-    </row>
-    <row r="58" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="18"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="15" t="s">
+      <c r="G57" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H57" s="18">
+        <v>4.9564144892331082E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="14"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="E58" s="15" t="s">
+      <c r="E58" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="F58" s="15" t="s">
+      <c r="F58" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="G58" s="16"/>
-      <c r="H58" s="16"/>
-    </row>
-    <row r="59" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="15" t="s">
+      <c r="G58" s="10">
+        <v>4.9564144892331082E-2</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="14"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E59" s="15" t="s">
+      <c r="E59" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F59" s="15" t="s">
+      <c r="F59" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="G59" s="16"/>
-      <c r="H59" s="16"/>
-    </row>
-    <row r="60" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="15" t="s">
+      <c r="G59" s="10">
+        <v>0.28571458224201529</v>
+      </c>
+      <c r="H59" s="18">
+        <v>0.28571458224201529</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="E60" s="15" t="s">
+      <c r="E60" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="F60" s="15" t="s">
+      <c r="F60" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="G60" s="16"/>
-      <c r="H60" s="16"/>
-    </row>
-    <row r="61" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="15" t="s">
+      <c r="G60" s="10">
+        <v>1.70837358770701E-8</v>
+      </c>
+      <c r="H60" s="18">
+        <v>1.70837358770701E-8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="14"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E61" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F61" s="15" t="s">
+      <c r="F61" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="G61" s="16"/>
-      <c r="H61" s="16"/>
-    </row>
-    <row r="62" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18">
+      <c r="G61" s="10">
+        <v>8.8375991442979085E-2</v>
+      </c>
+      <c r="H61" s="18">
+        <v>8.8375991442979085E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="14">
         <v>13</v>
       </c>
-      <c r="B62" s="24" t="s">
+      <c r="B62" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E62" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="F62" s="15" t="s">
+      <c r="F62" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-    </row>
-    <row r="63" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18"/>
-      <c r="B63" s="24"/>
-      <c r="C63" s="15" t="s">
+      <c r="G62" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H62" s="18">
+        <v>0.36660701815092989</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="14"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="E63" s="15" t="s">
+      <c r="E63" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="F63" s="15" t="s">
+      <c r="F63" s="19" t="s">
         <v>279</v>
       </c>
-      <c r="G63" s="16"/>
-      <c r="H63" s="16"/>
-    </row>
-    <row r="64" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="15" t="s">
+      <c r="G63" s="10">
+        <v>0.36660701815092989</v>
+      </c>
+      <c r="H63" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="14"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="D64" s="19" t="s">
         <v>280</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E64" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="F64" s="15" t="s">
+      <c r="F64" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="G64" s="16"/>
-      <c r="H64" s="16"/>
-    </row>
-    <row r="65" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
-      <c r="B65" s="24"/>
-      <c r="C65" s="15" t="s">
+      <c r="G64" s="10">
+        <v>0.2243928592985632</v>
+      </c>
+      <c r="H64" s="18">
+        <v>0.2243928592985632</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="14"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D65" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="E65" s="15" t="s">
+      <c r="E65" s="19" t="s">
         <v>283</v>
       </c>
-      <c r="F65" s="15" t="s">
+      <c r="F65" s="19" t="s">
         <v>284</v>
       </c>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="15" t="s">
+      <c r="G65" s="10">
+        <v>3.6528230012796208E-8</v>
+      </c>
+      <c r="H65" s="18">
+        <v>3.6528230012796208E-8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="14"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D66" s="15" t="s">
+      <c r="D66" s="19" t="s">
         <v>285</v>
       </c>
-      <c r="E66" s="15" t="s">
+      <c r="E66" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="F66" s="15" t="s">
+      <c r="F66" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="G66" s="16"/>
-      <c r="H66" s="16"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="19"/>
-      <c r="C67" s="20"/>
-      <c r="G67" s="22"/>
-      <c r="H67" s="21"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="G68" s="23"/>
-      <c r="H68" s="21"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="19"/>
-      <c r="C69" s="20"/>
-      <c r="G69" s="23"/>
-      <c r="H69" s="21"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="19"/>
-      <c r="C70" s="20"/>
-      <c r="G70" s="23"/>
-      <c r="H70" s="21"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="19"/>
-      <c r="C71" s="20"/>
-      <c r="G71" s="23"/>
-      <c r="H71" s="21"/>
+      <c r="G66" s="10">
+        <v>0.69727124237058369</v>
+      </c>
+      <c r="H66" s="18">
+        <v>0.69727124237058369</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="14">
+        <v>14</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="H67" s="18">
+        <v>6.8929458397063922E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="14"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="G68" s="10">
+        <v>6.8929458397063922E-2</v>
+      </c>
+      <c r="H68" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="14"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="G69" s="10">
+        <v>2.9830623376591902E-6</v>
+      </c>
+      <c r="H69" s="18">
+        <v>2.9830623376591902E-6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="14"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="G70" s="10">
+        <v>1.392126825213835E-14</v>
+      </c>
+      <c r="H70" s="18">
+        <v>1.392126825213835E-14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="14"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="G71" s="10">
+        <v>7.0780265569183052E-3</v>
+      </c>
+      <c r="H71" s="18">
+        <v>7.0780265569183052E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B75" s="13"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="28">
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B47:B51"/>
     <mergeCell ref="B67:B71"/>
@@ -2933,6 +3439,7 @@
     <mergeCell ref="A12:A16"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A67:A71"/>
     <mergeCell ref="A52:A56"/>
     <mergeCell ref="A57:A61"/>
     <mergeCell ref="A62:A66"/>
@@ -2949,811 +3456,899 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB97FFD-4B99-4361-B6D3-1A364FD5B282}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="15" t="s">
+      <c r="G2" s="10">
+        <v>0.93675692091108853</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15" t="s">
+      <c r="G3" s="10">
+        <v>1.1892241064580051E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="16"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13">
+      <c r="G4" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="16"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15" t="s">
+      <c r="G5" s="10">
+        <v>3.2016677606426138E-10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="16"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="s">
+      <c r="G6" s="10">
+        <v>0.743532461668439</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="16"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="G7" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
         <v>3</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="16"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15" t="s">
+      <c r="G8" s="10">
+        <v>9.5814905429724194E-8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="16"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15" t="s">
+      <c r="G9" s="10">
+        <v>0.28530811081230639</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="16"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="13">
+      <c r="G10" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="17">
         <v>4</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15" t="s">
+      <c r="G11" s="10">
+        <v>3.9997776056548296E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15" t="s">
+      <c r="G12" s="10">
+        <v>0.38351106928310691</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="16"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
+      <c r="G13" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="17">
         <v>5</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="16"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="15" t="s">
+      <c r="G14" s="10">
+        <v>0.45458408472986112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15" t="s">
+      <c r="G15" s="10">
+        <v>0.44237835343467868</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="G16" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="17">
         <v>6</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="16"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15" t="s">
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15" t="s">
+      <c r="G18" s="10">
+        <v>1.1763004327896389E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="17"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+      <c r="G19" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="17">
         <v>7</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15" t="s">
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="17"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="15" t="s">
+      <c r="G21" s="10">
+        <v>0.1183057268373853</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="16"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="13">
+      <c r="G22" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="17">
         <v>8</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G23" s="16"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15" t="s">
+      <c r="G23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="17"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="G24" s="16"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15" t="s">
+      <c r="G24" s="10">
+        <v>0.57703240172647929</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="16"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="13">
+      <c r="G25" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="17">
         <v>9</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="G26" s="16"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15" t="s">
+      <c r="G26" s="10">
+        <v>0.34159908562343261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="G27" s="16"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15" t="s">
+      <c r="G27" s="10">
+        <v>2.1433147657244551E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
+      <c r="G28" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="17">
         <v>10</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="15" t="s">
+      <c r="D29" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="G29" s="16"/>
-    </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15" t="s">
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="G30" s="16"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15" t="s">
+      <c r="G30" s="10">
+        <v>3.8633414539437723E-5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="G31" s="16"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="13">
+      <c r="G31" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="17">
         <v>11</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="G32" s="16"/>
-    </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="15" t="s">
+      <c r="G32" s="10">
+        <v>0.39788891923977088</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G33" s="16"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="15" t="s">
+      <c r="G33" s="10">
+        <v>3.4481029855785098E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="G34" s="16"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="13">
+      <c r="G34" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="17">
         <v>12</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="16"/>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="15" t="s">
+      <c r="G35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="17"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="G36" s="16"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="15" t="s">
+      <c r="G36" s="10">
+        <v>2.182190128758563E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="17"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="16"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="13">
+      <c r="G37" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="17">
         <v>13</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="G38" s="16"/>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="15" t="s">
+      <c r="G38" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="17"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="G39" s="16"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="15" t="s">
+      <c r="G39" s="10">
+        <v>1.2543753298802369E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="17"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="G40" s="16"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
+      <c r="G40" s="10" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="17">
         <v>14</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="G41" s="16"/>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="15" t="s">
+      <c r="G41" s="10">
+        <v>0.31074943747754441</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="17"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="G42" s="16"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="15" t="s">
+      <c r="G42" s="10">
+        <v>1.5535257094264251E-8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="17"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="G43" s="16"/>
+      <c r="G43" s="10" t="s">
+        <v>312</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -3779,12 +4374,12 @@
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>